<commit_message>
adding data and files from Sat cooldown
</commit_message>
<xml_diff>
--- a/Physics108_BABYBLUE/connection_diagram.xlsx
+++ b/Physics108_BABYBLUE/connection_diagram.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="13">
   <si>
     <t>gnd</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>squid nv meas</t>
+  </si>
+  <si>
+    <t>squid return meas</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -625,12 +630,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -644,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>0</v>

</xml_diff>